<commit_message>
Der scheiß ist weiss
</commit_message>
<xml_diff>
--- a/data/catalogue_clean.xlsx
+++ b/data/catalogue_clean.xlsx
@@ -463,7 +463,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Im Festpreis von € sind sämtliche Leistungen einschließlich Softwarelizenzen Implementierung Schulungen und ein Jahr Wartung enthalten Weitere Kosten entstehen nur bei schriftlicher Beauftragung zusätzlicher Leistungen durch den Kunden</t>
+          <t>im festpreis von € sind sämtliche leistungen einschließlich softwarelizenzen implementierung schulungen und ein jahr wartung enthalten weitere kosten entstehen nur bei schriftlicher beauftragung zusätzlicher leistungen durch den kunden</t>
         </is>
       </c>
     </row>
@@ -480,7 +480,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Der Kunde zahlt eine monatliche Pauschale von € für bis zu 50 Benutzer Jede weitere gleichzeitige Benutzerlizenz wird mit 100 € pro Benutzer und Monat zusätzlich berechnet</t>
+          <t>der kunde zahlt eine monatliche pauschale von € für bis zu benutzer jede weitere gleichzeitige benutzerlizenz wird mit € pro benutzer und monat zusätzlich berechnet</t>
         </is>
       </c>
     </row>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Die Vergütung ist in drei Raten zahlbar 30 bei Projektbeginn 50 nach erfolgreicher Testinstallation und 20 nach finaler Abnahme der Gesamtleistung</t>
+          <t>die vergütung ist in drei raten zahlbar bei projektbeginn nach erfolgreicher testinstallation und nach finaler abnahme der gesamtleistung</t>
         </is>
       </c>
     </row>
@@ -514,7 +514,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Alle Preise verstehen sich in Euro zuzüglich gesetzlicher Mehrwertsteuer Rechnungen sind vom Kunden innerhalb von 30 Kalendertagen ab Rechnungsdatum ohne Abzug zu bezahlen</t>
+          <t>alle preise verstehen sich in euro zuzüglich gesetzlicher mehrwertsteuer rechnungen sind vom kunden innerhalb von kalendertagen ab rechnungsdatum ohne abzug zu bezahlen</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Reise und Übernachtungskosten werden nur erstattet wenn sie vom Kunden vorab genehmigt wurden und werden zum Selbstkostenpreis gegen Beleg abgerechnet Leistungen die über den vereinbarten Umfang hinausgehen dürfen vom Anbieter nur nach schriftlichem Auftrag des Kunden ausgeführt werden und werden nach Aufwand zu 120 €Std vergütet</t>
+          <t>reise und übernachtungskosten werden nur erstattet wenn sie vom kunden vorab genehmigt wurden und werden zum selbstkostenpreis gegen beleg abgerechnet leistungen die über den vereinbarten umfang hinausgehen dürfen vom anbieter nur nach schriftlichem auftrag des kunden ausgeführt werden und werden nach aufwand zu € std vergütet</t>
         </is>
       </c>
     </row>
@@ -548,7 +548,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Die monatliche Nutzungsgebühr ist für die ersten 24 Monate festgeschrieben Danach kann der Anbieter den Preis einmal jährlich entsprechend der Inflationsrate maximal jedoch um 5 pro Jahr erhöhen Eine Erhöhung ist dem Kunden mindestens 2 Monate im Voraus schriftlich anzukündigen</t>
+          <t>die monatliche nutzungsgebühr ist für die ersten monate festgeschrieben danach kann der anbieter den preis einmal jährlich entsprechend der inflationsrate maximal jedoch um pro jahr erhöhen eine erhöhung ist dem kunden mindestens monate im voraus schriftlich anzukündigen</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Die Parteien vereinbaren ein Höchstbudget von € für alle in diesem Vertrag beschriebenen Leistungen Eine Überschreitung dieses Budgets bedarf der vorherigen schriftlichen Zustimmung des Kunden</t>
+          <t>die parteien vereinbaren ein höchstbudget von € für alle in diesem vertrag beschriebenen leistungen eine überschreitung dieses budgets bedarf der vorherigen schriftlichen zustimmung des kunden</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Gerät der Kunde mit einer Zahlung in Verzug so werden Verzugszinsen in Höhe von 9 Prozentpunkten über dem Basiszinssatz pa fällig Bei einem Zahlungsverzug von mehr als 30 Tagen ist der Anbieter berechtigt seine Leistungen bis zum Ausgleich der offenen Beträge auszusetzen nachdem er den Kunden zuvor schriftlich gemahnt hat</t>
+          <t>gerät der kunde mit einer zahlung in verzug so werden verzugszinsen in höhe von prozentpunkten über dem basiszinssatz p a fällig bei einem zahlungsverzug von mehr als tagen ist der anbieter berechtigt seine leistungen bis zum ausgleich der offenen beträge auszusetzen nachdem er den kunden zuvor schriftlich gemahnt hat</t>
         </is>
       </c>
     </row>
@@ -599,7 +599,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Der Leistungsumfang umfasst die Einführung des ERPSystems XYZ in den Modulen Finanzen Warenwirtschaft und CRM gemäß der Funktionsbeschreibung in Anlage 1 Nicht enthalten sind darüberhinausgehende Funktionen oder Prozesse sofern sie nicht ausdrücklich schriftlich vereinbart wurden</t>
+          <t>der leistungsumfang umfasst die einführung des erp systems xyz in den modulen finanzen warenwirtschaft und crm gemäß der funktionsbeschreibung in anlage nicht enthalten sind darüberhinausgehende funktionen oder prozesse sofern sie nicht ausdrücklich schriftlich vereinbart wurden</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Der Anbieter liefert im Rahmen dieses Projekts folgende Leistungen Installation und Konfiguration der ERPSoftware in der aktuellen Version Entwicklung der Schnittstelle zum Webshop Migration der Altdaten Stammdaten und offene Posten zwei AdminSchulungen für die IT des Kunden sowie eine deutschsprachige Anwenderdokumentation</t>
+          <t>der anbieter liefert im rahmen dieses projekts folgende leistungen installation und konfiguration der erp software in der aktuellen version entwicklung der schnittstelle zum webshop migration der altdaten stammdaten und offene posten zwei admin schulungen für die it des kunden sowie eine deutschsprachige anwenderdokumentation</t>
         </is>
       </c>
     </row>
@@ -633,7 +633,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Das eingeführte System muss 100 gleichzeitige Nutzer ohne spürbare Performanceeinbußen unterstützen und unter Volllast Transaktionen innerhalb von 2 Sekunden verarbeiten Außerdem erfüllt die Software die relevanten gesetzlichen Anforderungen GoBDKonformität GDPdU DSGVO für den Einsatz im Finanzwesen</t>
+          <t>das eingeführte system muss gleichzeitige nutzer ohne spürbare performanceeinbußen unterstützen und unter volllast transaktionen innerhalb von sekunden verarbeiten außerdem erfüllt die software die relevanten gesetzlichen anforderungen gobd konformität gdpdu dsgvo für den einsatz im finanzwesen</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Nicht Bestandteil dieses Vertrags sind die Lieferung von Hardware die Bereitstellung von Datenbanklizenzen sowie Anpassungen am LegacyCRMSystem des Kunden Diese Leistungen liegen in der Verantwortung des Kunden bzw werden gesondert beauftragt</t>
+          <t>nicht bestandteil dieses vertrags sind die lieferung von hardware die bereitstellung von datenbanklizenzen sowie anpassungen am legacy crm system des kunden diese leistungen liegen in der verantwortung des kunden bzw werden gesondert beauftragt</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Im Leistungsumfang enthalten ist die Entwicklung einer bidirektionalen Schnittstelle zwischen dem ERPSystem und dem bestehenden Webshop des Kunden Über diese Schnittstelle werden Produktstammdaten und Bestelldaten täglich synchronisiert Die technischen Details sind in Anlage 2 beschrieben</t>
+          <t>im leistungsumfang enthalten ist die entwicklung einer bidirektionalen schnittstelle zwischen dem erp system und dem bestehenden webshop des kunden über diese schnittstelle werden produktstammdaten und bestelldaten täglich synchronisiert die technischen details sind in anlage beschrieben</t>
         </is>
       </c>
     </row>
@@ -684,7 +684,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Dem Vertrag liegt das vom Auftraggeber freigegebene Pflichtenheft Anlage 3 zugrunde in dem sämtliche fachlichen Anforderungen und Funktionen beschrieben sind Dieses Pflichtenheft wird Bestandteil des Vertrags und dient als Maßstab für die Leistungserbringung und Abnahme</t>
+          <t>dem vertrag liegt das vom auftraggeber freigegebene pflichtenheft anlage zugrunde in dem sämtliche fachlichen anforderungen und funktionen beschrieben sind dieses pflichtenheft wird bestandteil des vertrags und dient als maßstab für die leistungserbringung und abnahme</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Voraussetzung für die erfolgreiche Implementierung ist dass der Kunde eine geeignete ServerInfrastruktur Windows Server 2019 64 GB RAM 1 TB Speicher bereitstellt und die erforderlichen Testdaten in abgestimmter Qualität zur Verfügung stellt</t>
+          <t>voraussetzung für die erfolgreiche implementierung ist dass der kunde eine geeignete server infrastruktur windows server gb ram tb speicher bereitstellt und die erforderlichen testdaten in abgestimmter qualität zur verfügung stellt</t>
         </is>
       </c>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Der Projektzeitplan wird als Anlage 2 festgeschrieben Wichtige Meilensteine sind Abschluss der Konzeptphase bis 3103 Fertigstellung der Implementierung bis 3107 Beginn Integrationstest am 1508 GoLive zum 0110 Konkrete Meilensteinziele und termine sind dem Plan in Anlage 2 zu entnehmen</t>
+          <t>der projektzeitplan wird als anlage festgeschrieben wichtige meilensteine sind abschluss der konzeptphase bis fertigstellung der implementierung bis beginn integrationstest am go live zum konkrete meilensteinziele und termine sind dem plan in anlage zu entnehmen</t>
         </is>
       </c>
     </row>
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Meilenstein 3 – Abschluss Integrationstest Alle Schnittstellen zu den Umsystemen SAPFI Webshop sind implementiert und im Integrationstest erfolgreich geprüft siehe Testprotokoll Dieser Meilenstein gilt als erreicht wenn sämtliche im Testprotokoll aufgeführten Testszenarien erfolgreich durchgeführt wurden</t>
+          <t>meilenstein – abschluss integrationstest alle schnittstellen zu den umsystemen sap fi webshop sind implementiert und im integrationstest erfolgreich geprüft siehe testprotokoll dieser meilenstein gilt als erreicht wenn sämtliche im testprotokoll aufgeführten testszenarien erfolgreich durchgeführt wurden</t>
         </is>
       </c>
     </row>
@@ -752,7 +752,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Voraussetzung für den Abschluss der Phase Datenmigration Meilenstein M5 ist dass der Kunde bis zum 15 alle zu migrierenden Altdaten in dem mit dem Anbieter abgestimmten Format bereitstellt Kommt der Kunde dieser Mitwirkung nicht nach verlängern sich die betroffenen nachfolgenden Fristen angemessen</t>
+          <t>voraussetzung für den abschluss der phase datenmigration meilenstein m ist dass der kunde bis zum alle zu migrierenden altdaten in dem mit dem anbieter abgestimmten format bereitstellt kommt der kunde dieser mitwirkung nicht nach verlängern sich die betroffenen nachfolgenden fristen angemessen</t>
         </is>
       </c>
     </row>
@@ -769,7 +769,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Erkennt eine Partei dass vereinbarte Termine nicht gehalten werden können informiert sie unverzüglich die andere Seite unter Angabe der Gründe Die Parteien werden sodann einvernehmlich einen aktualisierten Projektplan erstellen Bei vom Anbieter zu vertretendem Verzug der finalen Abnahme um mehr als 30 Kalendertage zahlt der Anbieter an den Kunden eine Vertragsstrafe von 05 der Gesamtsumme pro weiterer angefangener Verzugswoche maximal jedoch 5 der Gesamtsumme</t>
+          <t>erkennt eine partei dass vereinbarte termine nicht gehalten werden können informiert sie unverzüglich die andere seite unter angabe der gründe die parteien werden sodann einvernehmlich einen aktualisierten projektplan erstellen bei vom anbieter zu vertretendem verzug der finalen abnahme um mehr als kalendertage zahlt der anbieter an den kunden eine vertragsstrafe von der gesamtsumme pro weiterer angefangener verzugswoche maximal jedoch der gesamtsumme</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Die Projektparteien führen mindestens alle 14 Tage ein JourfixeMeeting zur Projektabstimmung durch vor Ort oder via Webkonferenz Zusätzlich erstellt der Anbieter zum Monatsende einen schriftlichen Projektstatusbericht der den Arbeitsfortschritt eventuelle ProblemeRisiken und den Erfüllungsgrad der Meilensteine darlegt Besprechungsergebnisse gelten als anerkannt wenn der Kunde nicht innerhalb von 5 Werktagen schriftlich widerspricht</t>
+          <t>die projektparteien führen mindestens alle tage ein jour fixe meeting zur projektabstimmung durch vor ort oder via webkonferenz zusätzlich erstellt der anbieter zum monatsende einen schriftlichen projektstatusbericht der den arbeitsfortschritt eventuelle probleme risiken und den erfüllungsgrad der meilensteine darlegt besprechungsergebnisse gelten als anerkannt wenn der kunde nicht innerhalb von werktagen schriftlich widerspricht</t>
         </is>
       </c>
     </row>
@@ -803,7 +803,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Nach Fertigstellung der jeweiligen Leistung informiert der Anbieter den Kunden schriftlich und fordert ihn zur Abnahme auf Der Kunde führt innerhalb von 10 Werktagen die Abnahmetests gemäß Abnahmeplan Anlage 4 durch Sind die vereinbarten Abnahmekriterien erfüllt erklärt der Kunde schriftlich die Abnahme der Leistung gegenüber dem Anbieter</t>
+          <t>nach fertigstellung der jeweiligen leistung informiert der anbieter den kunden schriftlich und fordert ihn zur abnahme auf der kunde führt innerhalb von werktagen die abnahmetests gemäß abnahmeplan anlage durch sind die vereinbarten abnahmekriterien erfüllt erklärt der kunde schriftlich die abnahme der leistung gegenüber dem anbieter</t>
         </is>
       </c>
     </row>
@@ -820,7 +820,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Abnahmekriterium für das Gesamtsystem ist die vollständige Erfüllung aller als ‚Muss‘ gekennzeichneten Anforderungen im Pflichtenheft sowie der erfolgreiche Abschluss aller im AbnahmeTestplan definierten Tests ohne kritische Fehler Fehlerklasse 1</t>
+          <t>abnahmekriterium für das gesamtsystem ist die vollständige erfüllung aller als ‚muss‘ gekennzeichneten anforderungen im pflichtenheft sowie der erfolgreiche abschluss aller im abnahme testplan definierten tests ohne kritische fehler fehlerklasse</t>
         </is>
       </c>
     </row>
@@ -837,7 +837,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Der Kunde wird die vom Anbieter zur Abnahme gestellte Leistung innerhalb von 15 Werktagen testen und schriftlich die Abnahme erklären oder bis dahin aufgetretene wesentliche Mängel schriftlich anzeigen Lässt der Kunde diese Frist verstreichen gilt die Leistung als abgenommen</t>
+          <t>der kunde wird die vom anbieter zur abnahme gestellte leistung innerhalb von werktagen testen und schriftlich die abnahme erklären oder bis dahin aufgetretene wesentliche mängel schriftlich anzeigen lässt der kunde diese frist verstreichen gilt die leistung als abgenommen</t>
         </is>
       </c>
     </row>
@@ -854,7 +854,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Die Implementierung jeder Modulgruppe wird vom Kunden unmittelbar nach Fertigstellung einer Teilabnahme unterzogen Nach erfolgreicher Teilabnahme eines Moduls gelten dessen Funktionen als vertragsgerecht geliefert Die Schlussabnahme des Gesamtprojekts erfolgt nach Abschluss aller Leistungen bereits teilabgenommene Leistungen werden dabei nur auf ihr Zusammenspiel hin überprüft</t>
+          <t>die implementierung jeder modulgruppe wird vom kunden unmittelbar nach fertigstellung einer teilabnahme unterzogen nach erfolgreicher teilabnahme eines moduls gelten dessen funktionen als vertragsgerecht geliefert die schlussabnahme des gesamtprojekts erfolgt nach abschluss aller leistungen bereits teilabgenommene leistungen werden dabei nur auf ihr zusammenspiel hin überprüft</t>
         </is>
       </c>
     </row>
@@ -871,7 +871,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Verweigert der Kunde die Abnahme wegen erheblicher Mängel so wird der Anbieter diese Mängel innerhalb von 15 Werktagen beheben und die Leistung erneut zur Abnahme vorlegen Die Abnahme darf bei geringfügigen Mängeln die den Vertragszweck nicht wesentlich beeinträchtigen nicht verweigert werden solche Mängel wird der Anbieter im Rahmen der Gewährleistung unverzüglich beseitigen</t>
+          <t>verweigert der kunde die abnahme wegen erheblicher mängel so wird der anbieter diese mängel innerhalb von werktagen beheben und die leistung erneut zur abnahme vorlegen die abnahme darf bei geringfügigen mängeln die den vertragszweck nicht wesentlich beeinträchtigen nicht verweigert werden solche mängel wird der anbieter im rahmen der gewährleistung unverzüglich beseitigen</t>
         </is>
       </c>
     </row>
@@ -888,7 +888,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Nimmt der Kunde die Leistung nicht innerhalb von 10 Werktagen nach Bereitstellung ab und nennt er innerhalb dieser Frist keine die Abnahme hindernden Mängel oder hat er die Software bereits produktiv in Gebrauch genommen so gilt die Leistung als abgenommen</t>
+          <t>nimmt der kunde die leistung nicht innerhalb von werktagen nach bereitstellung ab und nennt er innerhalb dieser frist keine die abnahme hindernden mängel oder hat er die software bereits produktiv in gebrauch genommen so gilt die leistung als abgenommen</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Mit der Abnahme der Gesamtleistung durch den Kunden gelten die vertraglichen Leistungen als erfüllt Damit wird die letzte Rate in Höhe von € zur Zahlung fällig Ab diesem Zeitpunkt beginnt die zwölfmonatige Gewährleistungsfrist gemäß § 10 dieses Vertrags</t>
+          <t>mit der abnahme der gesamtleistung durch den kunden gelten die vertraglichen leistungen als erfüllt damit wird die letzte rate in höhe von € zur zahlung fällig ab diesem zeitpunkt beginnt die zwölfmonatige gewährleistungsfrist gemäß § dieses vertrags</t>
         </is>
       </c>
     </row>
@@ -922,7 +922,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Der Anbieter sichert eine Verfügbarkeit des CloudServices von 995 im Jahresmittel zu Zeiten geplanter Wartungsfenster gemäß Abschnitt 5 werden bei der Berechnung nicht als Ausfall gewertet</t>
+          <t>der anbieter sichert eine verfügbarkeit des cloud services von im jahresmittel zu zeiten geplanter wartungsfenster gemäß abschnitt werden bei der berechnung nicht als ausfall gewertet</t>
         </is>
       </c>
     </row>
@@ -939,7 +939,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Supportfälle werden wie folgt priorisiert Kritisch System nicht verfügbar – Reaktionszeit 1 Stunde Lösungsziel 8 Stunden Hoch wesentliche Funktion gestört – Reaktion 4 Std Lösung innerhalb 2 Werktagen Niedrig geringfügige Beeinträchtigung – Reaktion 1 Werktag Lösung mit dem nächsten Update Diese Zeiten gelten während der Supportzeiten Mo–Fr 8–18 Uhr</t>
+          <t>supportfälle werden wie folgt priorisiert kritisch system nicht verfügbar – reaktionszeit stunde lösungsziel stunden hoch wesentliche funktion gestört – reaktion std lösung innerhalb werktagen niedrig geringfügige beeinträchtigung – reaktion werktag lösung mit dem nächsten update diese zeiten gelten während der supportzeiten mo–fr – uhr</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Regelmäßige Wartungen finden einmal pro Monat sonntags zwischen 0200 und 0500 Uhr statt In dieser Zeit kann der Service vorübergehend nicht verfügbar sein Der Anbieter wird außerplanmäßige Wartungsarbeiten mindestens 5 Werktage im Voraus ankündigen und nach Möglichkeit nachts oder am Wochenende durchführen</t>
+          <t>regelmäßige wartungen finden einmal pro monat sonntags zwischen und uhr statt in dieser zeit kann der service vorübergehend nicht verfügbar sein der anbieter wird außerplanmäßige wartungsarbeiten mindestens werktage im voraus ankündigen und nach möglichkeit nachts oder am wochenende durchführen</t>
         </is>
       </c>
     </row>
@@ -973,7 +973,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Wird die zugesicherte Monatsverfügbarkeit unterschritten erhält der Kunde eine Gutschrift 5 der Monatsgebühr bei 99 10 bei 97 Unterschreitet die Verfügbarkeit 95 oder verletzt der Anbieter zum dritten Mal in Folge eine SLAVorgabe erheblich hat der Kunde das Recht den Vertrag außerordentlich zu kündigen</t>
+          <t>wird die zugesicherte monatsverfügbarkeit unterschritten erhält der kunde eine gutschrift der monatsgebühr bei bei unterschreitet die verfügbarkeit oder verletzt der anbieter zum dritten mal in folge eine sla vorgabe erheblich hat der kunde das recht den vertrag außerordentlich zu kündigen</t>
         </is>
       </c>
     </row>
@@ -990,7 +990,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Der Anbieter leistet technischen Support für den Kunden montags bis freitags von 0800–1800 Uhr MEZ per TelefonHotline und EMail in deutscher Sprache Außerhalb dieser Zeiten wird ein Notfallsupport per EMail in englischer Sprache mit Reaktionszeiten bis zu 8 Stunden angeboten</t>
+          <t>der anbieter leistet technischen support für den kunden montags bis freitags von – uhr mez per telefon hotline und e mail in deutscher sprache außerhalb dieser zeiten wird ein notfallsupport per e mail in englischer sprache mit reaktionszeiten bis zu stunden angeboten</t>
         </is>
       </c>
     </row>
@@ -1007,7 +1007,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Der Anbieter erstellt täglich automatisierte Backups aller Kundendaten und bewahrt diese mindestens 14 Tage auf Im Falle eines schwerwiegenden Systemausfalls beträgt die maximale Wiederanlaufzeit RTO 8 Stunden Ein Datenverlust von maximal 24 Stunden wird vom Kunden als tolerierbar akzeptiert RPO 24h</t>
+          <t>der anbieter erstellt täglich automatisierte backups aller kundendaten und bewahrt diese mindestens tage auf im falle eines schwerwiegenden systemausfalls beträgt die maximale wiederanlaufzeit rto stunden ein datenverlust von maximal stunden wird vom kunden als tolerierbar akzeptiert rpo h</t>
         </is>
       </c>
     </row>
@@ -1024,7 +1024,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Die Parteien schließen vor Leistungsbeginn eine Vereinbarung zur Auftragsverarbeitung gemäß Art 28 DSGVO die dieser Vereinbarung als Anlage beiliegt Darin werden ua Umfang Dauer Art und Zweck der Verarbeitung sowie die vom Anbieter einzuhaltenden technischen und organisatorischen Maßnahmen geregelt</t>
+          <t>die parteien schließen vor leistungsbeginn eine vereinbarung zur auftragsverarbeitung gemäß art dsgvo die dieser vereinbarung als anlage beiliegt darin werden u a umfang dauer art und zweck der verarbeitung sowie die vom anbieter einzuhaltenden technischen und organisatorischen maßnahmen geregelt</t>
         </is>
       </c>
     </row>
@@ -1041,7 +1041,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Der Anbieter speichert und verarbeitet Kundendaten ausschließlich auf Servern in Deutschland Eine Verlagerung der Daten in ein Land außerhalb der EUEWR erfolgt nur nach vorheriger schriftlicher Zustimmung des Kunden und unter Beachtung der gesetzlichen Vorgaben zB Abschluss der EUStandarddatenschutzklauseln</t>
+          <t>der anbieter speichert und verarbeitet kundendaten ausschließlich auf servern in deutschland eine verlagerung der daten in ein land außerhalb der eu ewr erfolgt nur nach vorheriger schriftlicher zustimmung des kunden und unter beachtung der gesetzlichen vorgaben z b abschluss der eu standarddatenschutzklauseln</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Die Parteien verpflichten sich alle ihnen im Rahmen dieses Vertrags zugänglich werdenden vertraulichen Informationen streng vertraulich zu behandeln und ausschließlich für die vertraglich vorgesehenen Zwecke zu verwenden Diese Geheimhaltungspflicht gilt über die Beendigung des Vertrags hinaus fort Als vertraulich gelten insbesondere Geschäfts und Betriebsgeheimnisse Kundendaten sowie technische Informationen des jeweils anderen</t>
+          <t>die parteien verpflichten sich alle ihnen im rahmen dieses vertrags zugänglich werdenden vertraulichen informationen streng vertraulich zu behandeln und ausschließlich für die vertraglich vorgesehenen zwecke zu verwenden diese geheimhaltungspflicht gilt über die beendigung des vertrags hinaus fort als vertraulich gelten insbesondere geschäfts und betriebsgeheimnisse kundendaten sowie technische informationen des jeweils anderen</t>
         </is>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Der Anbieter gewährleistet den Schutz der Kundendaten nach dem Stand der Technik Insbesondere werden alle Datenübertragungen per TLS verschlüsselt sensible Daten verschlüsselt gespeichert Rechenzentren sind ISOIEC 27001zertifiziert und durch Firewalls sowie IntrusionDetectionSysteme gesichert Sicherheitsupdates der Server erfolgen unverzüglich nach Verfügbarkeit</t>
+          <t>der anbieter gewährleistet den schutz der kundendaten nach dem stand der technik insbesondere werden alle datenübertragungen per tls verschlüsselt sensible daten verschlüsselt gespeichert rechenzentren sind iso iec zertifiziert und durch firewalls sowie intrusion detection systeme gesichert sicherheitsupdates der server erfolgen unverzüglich nach verfügbarkeit</t>
         </is>
       </c>
     </row>
@@ -1092,7 +1092,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Der Anbieter wird den Kunden unverzüglich schriftlich benachrichtigen sobald ihm eine Verletzung des Schutzes personenbezogener Kundendaten oder sonstiger sicherheitsrelevanter Vorfall bekannt wird Er wird alle erforderlichen Schritte unternehmen um die Auswirkungen zu minimieren und die Verletzung zu beheben und eng mit dem Kunden bei der Aufklärung und eventuellen Behördenmeldungen zusammenarbeiten</t>
+          <t>der anbieter wird den kunden unverzüglich schriftlich benachrichtigen sobald ihm eine verletzung des schutzes personenbezogener kundendaten oder sonstiger sicherheitsrelevanter vorfall bekannt wird er wird alle erforderlichen schritte unternehmen um die auswirkungen zu minimieren und die verletzung zu beheben und eng mit dem kunden bei der aufklärung und eventuellen behördenmeldungen zusammenarbeiten</t>
         </is>
       </c>
     </row>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Sämtliche Daten die der Kunde im Rahmen der Nutzung des Services eingibt oder generiert bleiben zu jeder Zeit Eigentum des Kunden Der Anbieter verwendet diese Daten ausschließlich zur Erfüllung seiner Leistungen aus diesem Vertrag Der Kunde kann jederzeit die Herausgabe einer aktuellen Kopie seiner Daten in einem gängigen Format verlangen</t>
+          <t>sämtliche daten die der kunde im rahmen der nutzung des services eingibt oder generiert bleiben zu jeder zeit eigentum des kunden der anbieter verwendet diese daten ausschließlich zur erfüllung seiner leistungen aus diesem vertrag der kunde kann jederzeit die herausgabe einer aktuellen kopie seiner daten in einem gängigen format verlangen</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Der Anbieter darf Subunternehmer zur Verarbeitung der Kundendaten einsetzen sofern er den Kunden vorab über deren Einsatz informiert Der Anbieter stellt sicher dass alle Subunternehmer vertraglich mindestens die gleichen Datenschutz und Datensicherheitsverpflichtungen einhalten wie er selbst Die Haftung des Anbieters bleibt von der Einschaltung von Subunternehmern unberührt</t>
+          <t>der anbieter darf subunternehmer zur verarbeitung der kundendaten einsetzen sofern er den kunden vorab über deren einsatz informiert der anbieter stellt sicher dass alle subunternehmer vertraglich mindestens die gleichen datenschutz und datensicherheitsverpflichtungen einhalten wie er selbst die haftung des anbieters bleibt von der einschaltung von subunternehmern unberührt</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Auf Verlangen des Kunden weist der Anbieter die Umsetzung der vereinbarten technischen und organisatorischen Sicherheitsmaßnahmen durch aktuelle Prüfzertifikate zB ISO 27001 oder Berichte unabhängiger Auditoren nach Alternativ darf der Kunde oder ein von ihm beauftragter zur Vertraulichkeit verpflichteter Dritter einmal jährlich während der üblichen Geschäftszeiten nach vorheriger Ankündigung ein Audit der relevanten Sicherheitsvorkehrungen des Anbieters durchführen</t>
+          <t>auf verlangen des kunden weist der anbieter die umsetzung der vereinbarten technischen und organisatorischen sicherheitsmaßnahmen durch aktuelle prüfzertifikate z b iso oder berichte unabhängiger auditoren nach alternativ darf der kunde oder ein von ihm beauftragter zur vertraulichkeit verpflichteter dritter einmal jährlich während der üblichen geschäftszeiten nach vorheriger ankündigung ein audit der relevanten sicherheitsvorkehrungen des anbieters durchführen</t>
         </is>
       </c>
     </row>
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Der Kunde stellt für die Projektdauer einen kompetenten Projektleiter und ausreichendes Fachpersonal KeyUser zur Verfügung Er wird dem Anbieter alle zur Leistungserbringung notwendigen Informationen und Unterlagen vollständig und rechtzeitig zur Verfügung stellen Entscheidungen oder Freigaben wird der Kunde binnen 5 Werktagen nach Vorlage treffen damit der Zeitplan eingehalten wird</t>
+          <t>der kunde stellt für die projektdauer einen kompetenten projektleiter und ausreichendes fachpersonal key user zur verfügung er wird dem anbieter alle zur leistungserbringung notwendigen informationen und unterlagen vollständig und rechtzeitig zur verfügung stellen entscheidungen oder freigaben wird der kunde binnen werktagen nach vorlage treffen damit der zeitplan eingehalten wird</t>
         </is>
       </c>
     </row>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Der Anbieter führt die vereinbarten Leistungen fachgerecht mit geschultem Personal und gemäß dem zum Zeitpunkt der Leistungserbringung allgemein anerkannten Stand der Technik durch Er gewährleistet die sorgfältige Planung und Umsetzung aller Aufgaben im Einklang mit dem Zeitplan vorausgesetzt der Kunde erbringt seine Mitwirkungspflichten wie vereinbart</t>
+          <t>der anbieter führt die vereinbarten leistungen fachgerecht mit geschultem personal und gemäß dem zum zeitpunkt der leistungserbringung allgemein anerkannten stand der technik durch er gewährleistet die sorgfältige planung und umsetzung aller aufgaben im einklang mit dem zeitplan vorausgesetzt der kunde erbringt seine mitwirkungspflichten wie vereinbart</t>
         </is>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Beide Vertragsparteien benennen jeweils einen Projektleiter als verbindlichen Ansprechpartner Wesentliche Projektentscheidungen werden im gemeinsamen Lenkungsausschuss getroffen der monatlich tagt Eskalationen Bei Streitigkeiten die auf Projektleiterebene nicht gelöst werden können wird der Lenkungsausschuss einberufen und entscheidet binnen 5 Werktagen</t>
+          <t>beide vertragsparteien benennen jeweils einen projektleiter als verbindlichen ansprechpartner wesentliche projektentscheidungen werden im gemeinsamen lenkungsausschuss getroffen der monatlich tagt eskalationen bei streitigkeiten die auf projektleiterebene nicht gelöst werden können wird der lenkungsausschuss einberufen und entscheidet binnen werktagen</t>
         </is>
       </c>
     </row>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Der Anbieter setzt für dieses Projekt Frau Müller als Projektleiterin und Herrn Schmidt als leitenden Entwickler ein Ein Austausch dieser Personen ist nur mit vorheriger schriftlicher Zustimmung des Kunden zulässig Der Anbieter wird im Falle eines genehmigten Wechsels sicherstellen dass die Ersatzperson vergleichbare Qualifikationen besitzt und in alle projektrelevanten Details eingearbeitet ist</t>
+          <t>der anbieter setzt für dieses projekt frau müller als projektleiterin und herrn schmidt als leitenden entwickler ein ein austausch dieser personen ist nur mit vorheriger schriftlicher zustimmung des kunden zulässig der anbieter wird im falle eines genehmigten wechsels sicherstellen dass die ersatzperson vergleichbare qualifikationen besitzt und in alle projektrelevanten details eingearbeitet ist</t>
         </is>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Der Kunde erhält das nicht ausschließliche Recht die vertragsgegenständliche Software in seinem Unternehmen auf bis zu 100 benannten Arbeitsplätzen zu nutzen Eine Weitergabe oder Zugänglichmachung der Software an Dritte ist nicht gestattet Das Nutzungsrecht ist zeitlich unbefristet und gilt weltweit für eigene Geschäftszwecke des Kunden</t>
+          <t>der kunde erhält das nicht ausschließliche recht die vertragsgegenständliche software in seinem unternehmen auf bis zu benannten arbeitsplätzen zu nutzen eine weitergabe oder zugänglichmachung der software an dritte ist nicht gestattet das nutzungsrecht ist zeitlich unbefristet und gilt weltweit für eigene geschäftszwecke des kunden</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Individuelle Entwicklungen die der Anbieter im Rahmen dieses Projekts erstellt zB kundenspezifische Erweiterungen Schnittstellen verbleiben im geistigen Eigentum des Anbieters Der Anbieter räumt dem Kunden jedoch ein zeitlich unbeschränktes unwiderrufliches und örtlich unbegrenztes Nutzungsrecht hieran für dessen interne Geschäftszwecke ein Dieses Nutzungsrecht umfasst auch das Recht den Quellcode für die Aufrechterhaltung der Nutzung durch den Kunden zu bearbeiten</t>
+          <t>individuelle entwicklungen die der anbieter im rahmen dieses projekts erstellt z b kundenspezifische erweiterungen schnittstellen verbleiben im geistigen eigentum des anbieters der anbieter räumt dem kunden jedoch ein zeitlich unbeschränktes unwiderrufliches und örtlich unbegrenztes nutzungsrecht hieran für dessen interne geschäftszwecke ein dieses nutzungsrecht umfasst auch das recht den quellcode für die aufrechterhaltung der nutzung durch den kunden zu bearbeiten</t>
         </is>
       </c>
     </row>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Der Anbieter stellt den Kunden von allen Forderungen Schäden und Aufwendungen frei die aus der Behauptung Dritter resultieren die vom Anbieter gelieferte Software verletze Schutzrechte Dritter Der Anbieter übernimmt die Kosten der Rechtsverteidigung und etwaige Vergleichszahlungen vorausgesetzt der Kunde informiert den Anbieter unverzüglich schriftlich über derartige Ansprüche und überlässt ihm die vollständige Kontrolle der Verteidigung Gelingt es dem Anbieter nicht dem Kunden die vertragsgemäße Nutzung der Software ohne Rechtsverletzung zu ermöglichen kann der Kunde den Vertrag aus wichtigem Grund kündigen</t>
+          <t>der anbieter stellt den kunden von allen forderungen schäden und aufwendungen frei die aus der behauptung dritter resultieren die vom anbieter gelieferte software verletze schutzrechte dritter der anbieter übernimmt die kosten der rechtsverteidigung und etwaige vergleichszahlungen vorausgesetzt der kunde informiert den anbieter unverzüglich schriftlich über derartige ansprüche und überlässt ihm die vollständige kontrolle der verteidigung gelingt es dem anbieter nicht dem kunden die vertragsgemäße nutzung der software ohne rechtsverletzung zu ermöglichen kann der kunde den vertrag aus wichtigem grund kündigen</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1279,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Der Anbieter ist berechtigt zur Erfüllung seiner Vertragspflichten Subunternehmer einzusetzen Die Einbindung von Subunternehmern entbindet den Anbieter nicht von seinen Pflichten gegenüber dem Kunden der Anbieter haftet für Handlungen und Unterlassungen seiner Subunternehmer wie für eigenes Verschulden Der Anbieter wird dem Kunden auf Wunsch die aktuell eingesetzten wesentlichen Subunternehmer benennen</t>
+          <t>der anbieter ist berechtigt zur erfüllung seiner vertragspflichten subunternehmer einzusetzen die einbindung von subunternehmern entbindet den anbieter nicht von seinen pflichten gegenüber dem kunden der anbieter haftet für handlungen und unterlassungen seiner subunternehmer wie für eigenes verschulden der anbieter wird dem kunden auf wunsch die aktuell eingesetzten wesentlichen subunternehmer benennen</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Der Anbieter darf den Kunden als Referenzkunden nennen ausschließlich Firmierung kein Logo und angeben dass der Kunde die Software des Anbieters einsetzt Weitergehende Öffentlichkeitsmaßnahmen zB Fallstudien Nutzung des Logos des Kunden bedürfen der vorherigen schriftlichen Zustimmung des Kunden</t>
+          <t>der anbieter darf den kunden als referenzkunden nennen ausschließlich firmierung kein logo und angeben dass der kunde die software des anbieters einsetzt weitergehende öffentlichkeitsmaßnahmen z b fallstudien nutzung des logos des kunden bedürfen der vorherigen schriftlichen zustimmung des kunden</t>
         </is>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Der Anbieter ist berechtigt maximal einmal pro Kalenderjahr die vertragsgemäße Nutzung der Software beim Kunden zu überprüfen Die Prüfung ist mindestens 2 Wochen vorher schriftlich anzukündigen und darf während der üblichen Geschäftszeiten erfolgen Mitarbeiter des Anbieters sind verpflichtet Betriebsgeheimnisse des Kunden vertraulich zu behandeln Erkennt die Prüfung eine Mehrnutzung wird der Kunde die zusätzliche Vergütung gemäß Vertrag nachentrichten</t>
+          <t>der anbieter ist berechtigt maximal einmal pro kalenderjahr die vertragsgemäße nutzung der software beim kunden zu überprüfen die prüfung ist mindestens wochen vorher schriftlich anzukündigen und darf während der üblichen geschäftszeiten erfolgen mitarbeiter des anbieters sind verpflichtet betriebsgeheimnisse des kunden vertraulich zu behandeln erkennt die prüfung eine mehrnutzung wird der kunde die zusätzliche vergütung gemäß vertrag nachentrichten</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Der Anbieter unterhält für die Laufzeit dieses Vertrages eine Haftpflichtversicherung Deckung mindestens 2 Mio € pro Schadensfall für Personen und Sachschäden 1 Mio € für Vermögensschäden Auf Verlangen weist der Anbieter dem Kunden den entsprechenden Versicherungsschutz nach Policenbescheinigung</t>
+          <t>der anbieter unterhält für die laufzeit dieses vertrages eine haftpflichtversicherung deckung mindestens mio € pro schadensfall für personen und sachschäden mio € für vermögensschäden auf verlangen weist der anbieter dem kunden den entsprechenden versicherungsschutz nach policenbescheinigung</t>
         </is>
       </c>
     </row>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Wünscht der Kunde Änderungen des vereinbarten Leistungsumfangs so wird er dem Anbieter einen schriftlichen Change Request mit Beschreibung der gewünschten Änderung übermitteln Der Anbieter prüft die Machbarkeit und Auswirkungen auf Vergütung und Zeitplan und unterbreitet dem Kunden ein Änderungsangebot Eine Umsetzung der Änderung erfolgt erst wenn beide Parteien dieses Angebot schriftlich genehmigt haben</t>
+          <t>wünscht der kunde änderungen des vereinbarten leistungsumfangs so wird er dem anbieter einen schriftlichen change request mit beschreibung der gewünschten änderung übermitteln der anbieter prüft die machbarkeit und auswirkungen auf vergütung und zeitplan und unterbreitet dem kunden ein änderungsangebot eine umsetzung der änderung erfolgt erst wenn beide parteien dieses angebot schriftlich genehmigt haben</t>
         </is>
       </c>
     </row>
@@ -1364,7 +1364,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Änderungen oder Ergänzungen dieses Vertrags – einschließlich einer Änderung des Leistungsumfangs – bedürfen zu ihrer Wirksamkeit der Schriftform und müssen von beiden Vertragsparteien unterzeichnet werden Mündliche Nebenabreden sind ausgeschlossen</t>
+          <t>änderungen oder ergänzungen dieses vertrags – einschließlich einer änderung des leistungsumfangs – bedürfen zu ihrer wirksamkeit der schriftform und müssen von beiden vertragsparteien unterzeichnet werden mündliche nebenabreden sind ausgeschlossen</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Für jede vereinbarte Leistungsänderung wird ein schriftliches ChangeOrderDokument erstellt Dieses enthält die Beschreibung der Änderung etwaige Mehr oder Minderleistungen die Anpassung des Zeitplans sowie die zusätzliche oder reduzierte Vergütung Das ChangeOrderDokument ist von beiden Parteien zu unterzeichnen und wird Bestandteil des Vertrags</t>
+          <t>für jede vereinbarte leistungsänderung wird ein schriftliches change order dokument erstellt dieses enthält die beschreibung der änderung etwaige mehr oder minderleistungen die anpassung des zeitplans sowie die zusätzliche oder reduzierte vergütung das change order dokument ist von beiden parteien zu unterzeichnen und wird bestandteil des vertrags</t>
         </is>
       </c>
     </row>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Der Kunde kann während der Projektdauer Änderungen oder Ergänzungen des vereinbarten Leistungsumfangs verlangen soweit diese dem Anbieter zumutbar sind Der Anbieter wird ein solches Verlangen prüfen Können sich die Parteien nicht binnen 10 Werktagen über die Umsetzung insb über Mehrkosten oder eine Terminverschiebung einigen entscheidet auf Wunsch des Kunden ein unabhängiger Gutachter über die Zumutbarkeit Das Recht des Kunden erforderlichenfalls gerichtlich die Anpassung des Vertrages zu verlangen bleibt unberührt</t>
+          <t>der kunde kann während der projektdauer änderungen oder ergänzungen des vereinbarten leistungsumfangs verlangen soweit diese dem anbieter zumutbar sind der anbieter wird ein solches verlangen prüfen können sich die parteien nicht binnen werktagen über die umsetzung insb über mehrkosten oder eine terminverschiebung einigen entscheidet auf wunsch des kunden ein unabhängiger gutachter über die zumutbarkeit das recht des kunden erforderlichenfalls gerichtlich die anpassung des vertrages zu verlangen bleibt unberührt</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Bei Beendigung des Vertrages stellt der Anbieter dem Kunden sämtliche vom Kunden stammenden Daten innerhalb von 10 Werktagen in einem gängigen maschinenlesbaren Format zB CSVDateien zur Verfügung Dies umfasst alle im System gespeicherten Stammdaten und Transaktionsdaten Die Datenübergabe ist für den Kunden mit keinen zusätzlichen Kosten verbunden</t>
+          <t>bei beendigung des vertrages stellt der anbieter dem kunden sämtliche vom kunden stammenden daten innerhalb von werktagen in einem gängigen maschinenlesbaren format z b csv dateien zur verfügung dies umfasst alle im system gespeicherten stammdaten und transaktionsdaten die datenübergabe ist für den kunden mit keinen zusätzlichen kosten verbunden</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Auf Wunsch des Kunden unterstützt der Anbieter die Transition der Services bei Vertragsbeendigung Insbesondere wird der Anbieter in den letzten zwei Vertragsmonaten bis zu 10 Personentage dafür einsetzen den Wechsel auf ein anderes System zu begleiten Datenexport Erläuterung der Systemkonfiguration Unterstützung des neuen Dienstleisters Diese Leistungen werden nach tatsächlich angefallenem Aufwand zu den vertraglich vereinbarten Tagessätzen vergütet</t>
+          <t>auf wunsch des kunden unterstützt der anbieter die transition der services bei vertragsbeendigung insbesondere wird der anbieter in den letzten zwei vertragsmonaten bis zu personentage dafür einsetzen den wechsel auf ein anderes system zu begleiten datenexport erläuterung der systemkonfiguration unterstützung des neuen dienstleisters diese leistungen werden nach tatsächlich angefallenem aufwand zu den vertraglich vereinbarten tagessätzen vergütet</t>
         </is>
       </c>
     </row>
@@ -1449,7 +1449,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Nach Vertragsbeendigung hält der Anbieter die Kundendaten noch für einen Zeitraum von 30 Tagen in der Produktivumgebung bereit Der Kunde hat in dieser Zeit weiterhin Lesezugriff auf das System um erforderliche Datenabzüge vorzunehmen Nach Ablauf der 30 Tage wird der Zugriff geschlossen</t>
+          <t>nach vertragsbeendigung hält der anbieter die kundendaten noch für einen zeitraum von tagen in der produktivumgebung bereit der kunde hat in dieser zeit weiterhin lesezugriff auf das system um erforderliche datenabzüge vorzunehmen nach ablauf der tage wird der zugriff geschlossen</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Der Anbieter wird 60 Tage nach Vertragsende sämtliche Kundendaten aus seinen Systemen und Backups unwiederbringlich löschen Auf schriftliches Verlangen des Kunden bestätigt der Anbieter die endgültige Löschung der Daten schriftlich bis spätestens 90 Tage nach Vertragsende</t>
+          <t>der anbieter wird tage nach vertragsende sämtliche kundendaten aus seinen systemen und backups unwiederbringlich löschen auf schriftliches verlangen des kunden bestätigt der anbieter die endgültige löschung der daten schriftlich bis spätestens tage nach vertragsende</t>
         </is>
       </c>
     </row>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Die Haftung des Anbieters aus und im Zusammenhang mit diesem Vertrag ist – außer in Fällen von Vorsatz oder grober Fahrlässigkeit – der Höhe nach je Vertragsjahr auf 100 der im jeweiligen Jahr vom Kunden gezahlten Vergütung maximal jedoch € begrenzt</t>
+          <t>die haftung des anbieters aus und im zusammenhang mit diesem vertrag ist – außer in fällen von vorsatz oder grober fahrlässigkeit – der höhe nach je vertragsjahr auf der im jeweiligen jahr vom kunden gezahlten vergütung maximal jedoch € begrenzt</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Der Anbieter haftet nicht für indirekte Schäden Folgeschäden oder entgangenen Gewinn des Kunden Von diesem Haftungsausschluss ausgenommen sind Schäden die auf Vorsatz oder grober Fahrlässigkeit des Anbieters beruhen</t>
+          <t>der anbieter haftet nicht für indirekte schäden folgeschäden oder entgangenen gewinn des kunden von diesem haftungsausschluss ausgenommen sind schäden die auf vorsatz oder grober fahrlässigkeit des anbieters beruhen</t>
         </is>
       </c>
     </row>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Die vorstehenden Haftungsbeschränkungen gelten nicht bei Vorsatz oder grober Fahrlässigkeit im Falle der Verletzung von Leben Körper oder Gesundheit sowie bei Ansprüchen nach dem Produkthaftungsgesetz In diesen Fällen haftet der Anbieter nach den gesetzlichen Bestimmungen unbegrenzt</t>
+          <t>die vorstehenden haftungsbeschränkungen gelten nicht bei vorsatz oder grober fahrlässigkeit im falle der verletzung von leben körper oder gesundheit sowie bei ansprüchen nach dem produkthaftungsgesetz in diesen fällen haftet der anbieter nach den gesetzlichen bestimmungen unbegrenzt</t>
         </is>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Für Sachmängel beträgt die Gewährleistungsfrist 24 Monate ab Abnahme Für Rechtsmängel Verletzung Rechte Dritter gilt eine Verjährungsfrist von 36 Monaten ab Abnahme Sofern ein Mangel arglistig verschwiegen wurde gelten die gesetzlichen Fristen</t>
+          <t>für sachmängel beträgt die gewährleistungsfrist monate ab abnahme für rechtsmängel verletzung rechte dritter gilt eine verjährungsfrist von monaten ab abnahme sofern ein mangel arglistig verschwiegen wurde gelten die gesetzlichen fristen</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Treten während der Gewährleistungsfrist Mängel auf hat der Kunde diese dem Anbieter unverzüglich anzuzeigen Der Anbieter ist verpflichtet Sachmängel nach eigener Wahl durch Nachbesserung oder Austausch innerhalb angemessener Frist zu beheben Schlagen zwei Nacherfüllungsversuche fehl oder verzögert der Anbieter die Nacherfüllung unzumutbar kann der Kunde eine Herabsetzung der Vergütung Minderung verlangen oder – bei erheblichen Mängeln – vom Vertrag zurücktreten</t>
+          <t>treten während der gewährleistungsfrist mängel auf hat der kunde diese dem anbieter unverzüglich anzuzeigen der anbieter ist verpflichtet sachmängel nach eigener wahl durch nachbesserung oder austausch innerhalb angemessener frist zu beheben schlagen zwei nacherfüllungsversuche fehl oder verzögert der anbieter die nacherfüllung unzumutbar kann der kunde eine herabsetzung der vergütung minderung verlangen oder – bei erheblichen mängeln – vom vertrag zurücktreten</t>
         </is>
       </c>
     </row>
@@ -1568,7 +1568,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>HGB Untersuchungs und Rügepflicht findet auf die von diesem Vertrag umfassten Lieferungen keine Anwendung Die Mängelansprüche des Kunden bestimmen sich ausschließlich nach den Regelungen dieses Vertrags Abnahme und Gewährleistung</t>
+          <t>hgb untersuchungs und rügepflicht findet auf die von diesem vertrag umfassten lieferungen keine anwendung die mängelansprüche des kunden bestimmen sich ausschließlich nach den regelungen dieses vertrags abnahme und gewährleistung</t>
         </is>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Dieser Vertrag tritt am 01 in Kraft und hat eine feste Laufzeit bis zum 30062027 Während dieser Mindestlaufzeit ist eine ordentliche Kündigung ausgeschlossen</t>
+          <t>dieser vertrag tritt am in kraft und hat eine feste laufzeit bis zum während dieser mindestlaufzeit ist eine ordentliche kündigung ausgeschlossen</t>
         </is>
       </c>
     </row>
@@ -1602,7 +1602,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Nach Ablauf der Mindestlaufzeit von 24 Monaten verlängert sich der Vertrag jeweils automatisch um weitere 12 Monate sofern nicht eine Partei spätestens 3 Monate vor dem jeweiligen Vertragsende schriftlich kündigt Der Anbieter wird den Kunden spätestens 60 Tage vor Fristablauf auf das Kündigungsrecht hinweisen</t>
+          <t>nach ablauf der mindestlaufzeit von monaten verlängert sich der vertrag jeweils automatisch um weitere monate sofern nicht eine partei spätestens monate vor dem jeweiligen vertragsende schriftlich kündigt der anbieter wird den kunden spätestens tage vor fristablauf auf das kündigungsrecht hinweisen</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Das Recht zur Kündigung aus wichtigem Grund bleibt unberührt Ein wichtiger Grund liegt für den Kunden insbesondere vor wenn der Anbieter trotz schriftlicher Abmahnung wiederholt oder grob gegen wesentliche Vertragspflichten verstößt oder wenn über das Vermögen des Anbieters ein Insolvenzverfahren eröffnet wird In solchen Fällen kann der Kunde den Vertrag fristlos kündigen</t>
+          <t>das recht zur kündigung aus wichtigem grund bleibt unberührt ein wichtiger grund liegt für den kunden insbesondere vor wenn der anbieter trotz schriftlicher abmahnung wiederholt oder grob gegen wesentliche vertragspflichten verstößt oder wenn über das vermögen des anbieters ein insolvenzverfahren eröffnet wird in solchen fällen kann der kunde den vertrag fristlos kündigen</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Endet der Vertrag vor Ablauf eines bereits im Voraus bezahlten Leistungszeitraums erstattet der Anbieter dem Kunden die nicht verbrauchten Entgelte zeitanteilig Dies gilt nicht wenn der Kunde den wichtigen Grund für die außerordentliche Kündigung gesetzt hat in diesem Fall entfällt eine Erstattung</t>
+          <t>endet der vertrag vor ablauf eines bereits im voraus bezahlten leistungszeitraums erstattet der anbieter dem kunden die nicht verbrauchten entgelte zeitanteilig dies gilt nicht wenn der kunde den wichtigen grund für die außerordentliche kündigung gesetzt hat in diesem fall entfällt eine erstattung</t>
         </is>
       </c>
     </row>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Eine Übertragung von Rechten und Pflichten aus diesem Vertrag durch den Kunden auf Dritte bedarf der vorherigen schriftlichen Zustimmung des Anbieters Der Anbieter ist berechtigt diesen Vertrag mit einer Frist von 4 Wochen auf ein mit ihm konzernverbundenes Unternehmen zu übertragen der Kunde kann in diesem Fall den Vertrag zum Übergabezeitpunkt außerordentlich kündigen</t>
+          <t>eine übertragung von rechten und pflichten aus diesem vertrag durch den kunden auf dritte bedarf der vorherigen schriftlichen zustimmung des anbieters der anbieter ist berechtigt diesen vertrag mit einer frist von wochen auf ein mit ihm konzernverbundenes unternehmen zu übertragen der kunde kann in diesem fall den vertrag zum übergabezeitpunkt außerordentlich kündigen</t>
         </is>
       </c>
     </row>
@@ -1670,7 +1670,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Dieser Vertrag unterliegt dem Recht der Bundesrepublik Deutschland Das Übereinkommen der Vereinten Nationen über Verträge über den internationalen Warenkauf UNKaufrecht ist ausgeschlossen</t>
+          <t>dieser vertrag unterliegt dem recht der bundesrepublik deutschland das übereinkommen der vereinten nationen über verträge über den internationalen warenkauf un kaufrecht ist ausgeschlossen</t>
         </is>
       </c>
     </row>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Gerichtsstand für alle Streitigkeiten aus oder im Zusammenhang mit diesem Vertrag ist – soweit gesetzlich zulässig – München Deutschland</t>
+          <t>gerichtsstand für alle streitigkeiten aus oder im zusammenhang mit diesem vertrag ist – soweit gesetzlich zulässig – münchen deutschland</t>
         </is>
       </c>
     </row>
@@ -1704,7 +1704,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Dieser Vertrag wird in deutscher und englischer Sprache geschlossen Im Falle von Abweichungen zwischen den beiden Fassungen hat die deutsche Fassung Vorrang</t>
+          <t>dieser vertrag wird in deutscher und englischer sprache geschlossen im falle von abweichungen zwischen den beiden fassungen hat die deutsche fassung vorrang</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Sollte eine Bestimmung dieses Vertrages unwirksam oder undurchführbar sein oder werden bleibt die Wirksamkeit der übrigen Bestimmungen hiervon unberührt Die Parteien werden die unwirksame Bestimmung einvernehmlich durch eine solche Regelung ersetzen die dem wirtschaftlichen Zweck der unwirksamen Bestimmung am nächsten kommt</t>
+          <t>sollte eine bestimmung dieses vertrages unwirksam oder undurchführbar sein oder werden bleibt die wirksamkeit der übrigen bestimmungen hiervon unberührt die parteien werden die unwirksame bestimmung einvernehmlich durch eine solche regelung ersetzen die dem wirtschaftlichen zweck der unwirksamen bestimmung am nächsten kommt</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1738,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Keine der Parteien haftet für die Nichterfüllung ihrer vertraglichen Pflichten sofern höhere Gewalt die Erfüllung verhindert Als höhere Gewalt gelten Ereignisse die außerhalb der zumutbaren Kontrolle der Parteien liegen insbesondere Naturkatastrophen Krieg Terror staatliche Eingriffe oder Pandemien Jede Partei wird die andere unverzüglich über das Eintreten eines Falles höherer Gewalt informieren Dauert das Ereignis länger als 60 Tage an sind beide Parteien berechtigt den Vertrag außerordentlich zu kündigen</t>
+          <t>keine der parteien haftet für die nichterfüllung ihrer vertraglichen pflichten sofern höhere gewalt die erfüllung verhindert als höhere gewalt gelten ereignisse die außerhalb der zumutbaren kontrolle der parteien liegen insbesondere naturkatastrophen krieg terror staatliche eingriffe oder pandemien jede partei wird die andere unverzüglich über das eintreten eines falles höherer gewalt informieren dauert das ereignis länger als tage an sind beide parteien berechtigt den vertrag außerordentlich zu kündigen</t>
         </is>
       </c>
     </row>

</xml_diff>